<commit_message>
updated items and data file
</commit_message>
<xml_diff>
--- a/iifd_judgment_cards_task_items.xlsx
+++ b/iifd_judgment_cards_task_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/red/Documents/GitHub/iifd-judgment-cards-french/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713225D8-B0BC-2C42-86DC-A65B4E6ABB2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D22F435-6EDC-1849-9B6A-73AD118F9B9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="1560" windowWidth="22560" windowHeight="9780" firstSheet="14" activeTab="21" xr2:uid="{5FD661D1-94D7-7B43-9C52-59526989F8CE}"/>
+    <workbookView xWindow="1300" yWindow="440" windowWidth="24920" windowHeight="15680" xr2:uid="{5FD661D1-94D7-7B43-9C52-59526989F8CE}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline (D3)" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,17 @@
     <sheet name="control-false-none (E1)" sheetId="10" r:id="rId10"/>
     <sheet name="control-true (D1)" sheetId="17" r:id="rId11"/>
     <sheet name="control-true (E4)" sheetId="18" r:id="rId12"/>
-    <sheet name="critical-1 (B3)" sheetId="19" r:id="rId13"/>
-    <sheet name="critical-2 (A3)" sheetId="20" r:id="rId14"/>
-    <sheet name="critical-2 (A5)" sheetId="21" r:id="rId15"/>
-    <sheet name="critical-2 (C2)" sheetId="22" r:id="rId16"/>
-    <sheet name="critical-2 (C3)" sheetId="23" r:id="rId17"/>
-    <sheet name="critical-3 (A1)" sheetId="11" r:id="rId18"/>
-    <sheet name="critical-3 (A2)" sheetId="12" r:id="rId19"/>
-    <sheet name="critical-3 (C4)" sheetId="13" r:id="rId20"/>
-    <sheet name="critical-3 (C5)" sheetId="14" r:id="rId21"/>
-    <sheet name="practice" sheetId="15" r:id="rId22"/>
+    <sheet name="critical-1 (B3) (1,2 of 4)" sheetId="19" r:id="rId13"/>
+    <sheet name="critical-1 (B3) (3,4 of 4)" sheetId="24" r:id="rId14"/>
+    <sheet name="critical-2 (A3)" sheetId="20" r:id="rId15"/>
+    <sheet name="critical-2 (A5)" sheetId="21" r:id="rId16"/>
+    <sheet name="critical-2 (C2)" sheetId="22" r:id="rId17"/>
+    <sheet name="critical-2 (C3)" sheetId="23" r:id="rId18"/>
+    <sheet name="critical-3 (A1)" sheetId="11" r:id="rId19"/>
+    <sheet name="critical-3 (A2)" sheetId="12" r:id="rId20"/>
+    <sheet name="critical-3 (C4)" sheetId="13" r:id="rId21"/>
+    <sheet name="critical-3 (C5)" sheetId="14" r:id="rId22"/>
+    <sheet name="practice" sheetId="15" r:id="rId23"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6322" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6346" uniqueCount="903">
   <si>
     <t>Item</t>
   </si>
@@ -3133,7 +3134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09248CCD-A6D8-894F-AEC7-50874A02F112}">
   <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -6802,10 +6803,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C49919-EE7E-BB4C-832C-FBBD07F0738D}">
-  <dimension ref="A1:X25"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K25"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7045,55 +7046,55 @@
         <v>76</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>270</v>
+        <v>471</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>261</v>
+        <v>475</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>224</v>
+        <v>470</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>231</v>
+        <v>131</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>270</v>
+        <v>471</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>261</v>
+        <v>475</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>224</v>
+        <v>470</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>231</v>
+        <v>131</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>330</v>
+        <v>473</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>302</v>
@@ -7105,10 +7106,10 @@
         <v>300</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -7119,70 +7120,70 @@
         <v>76</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>134</v>
+        <v>188</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>135</v>
+        <v>187</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>216</v>
+        <v>412</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>215</v>
+        <v>411</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>134</v>
+        <v>188</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>135</v>
+        <v>187</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>216</v>
+        <v>412</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>215</v>
+        <v>411</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>283</v>
+        <v>414</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>303</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -7193,64 +7194,64 @@
         <v>76</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>471</v>
+        <v>199</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>475</v>
+        <v>198</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>470</v>
+        <v>182</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>132</v>
+        <v>248</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>131</v>
+        <v>216</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>471</v>
+        <v>199</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>475</v>
+        <v>198</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>470</v>
+        <v>182</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>132</v>
+        <v>248</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>131</v>
+        <v>216</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>473</v>
+        <v>289</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>313</v>
+        <v>283</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>303</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="W6" s="3" t="s">
         <v>302</v>
@@ -7267,70 +7268,70 @@
         <v>76</v>
       </c>
       <c r="C7" s="1">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>188</v>
+        <v>253</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>187</v>
+        <v>254</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>412</v>
+        <v>273</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>411</v>
+        <v>129</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>188</v>
+        <v>253</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>187</v>
+        <v>254</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>412</v>
+        <v>273</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>411</v>
+        <v>129</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>324</v>
+        <v>297</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>414</v>
+        <v>312</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>302</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
@@ -7341,61 +7342,61 @@
         <v>76</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>692</v>
+        <v>698</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>336</v>
+        <v>249</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>267</v>
+        <v>181</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>168</v>
+        <v>204</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>335</v>
+        <v>140</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>668</v>
+        <v>674</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>336</v>
+        <v>249</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>267</v>
+        <v>181</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>168</v>
+        <v>204</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>335</v>
+        <v>140</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>310</v>
+        <v>285</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>302</v>
@@ -7404,7 +7405,7 @@
         <v>301</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
@@ -7415,70 +7416,70 @@
         <v>76</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>80</v>
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>693</v>
+        <v>699</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>225</v>
+        <v>471</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>189</v>
+        <v>474</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>150</v>
+        <v>470</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>226</v>
+        <v>177</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>669</v>
+        <v>675</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>225</v>
+        <v>471</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>189</v>
+        <v>474</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>150</v>
+        <v>470</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>226</v>
+        <v>177</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>316</v>
+        <v>473</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="W9" s="3" t="s">
         <v>300</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
@@ -7489,67 +7490,67 @@
         <v>76</v>
       </c>
       <c r="C10" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>694</v>
+        <v>702</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>199</v>
+        <v>269</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>248</v>
+        <v>443</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>216</v>
+        <v>368</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>670</v>
+        <v>678</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>199</v>
+        <v>269</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>248</v>
+        <v>443</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>216</v>
+        <v>368</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>289</v>
+        <v>320</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>283</v>
+        <v>370</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>301</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="V10" s="1" t="s">
         <v>302</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="X10" s="3" t="s">
         <v>303</v>
@@ -7563,70 +7564,70 @@
         <v>76</v>
       </c>
       <c r="C11" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>695</v>
+        <v>703</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>253</v>
+        <v>223</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>254</v>
+        <v>224</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>129</v>
+        <v>202</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>671</v>
+        <v>679</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>253</v>
+        <v>223</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>254</v>
+        <v>224</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>129</v>
+        <v>202</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>297</v>
+        <v>330</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>301</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -7637,70 +7638,70 @@
         <v>76</v>
       </c>
       <c r="C12" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>696</v>
+        <v>706</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>412</v>
+        <v>209</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>410</v>
+        <v>211</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>442</v>
+        <v>210</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>430</v>
+        <v>255</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>426</v>
+        <v>253</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>672</v>
+        <v>682</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>412</v>
+        <v>209</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>410</v>
+        <v>211</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>442</v>
+        <v>210</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>430</v>
+        <v>255</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>426</v>
+        <v>253</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>414</v>
+        <v>328</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>428</v>
+        <v>297</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="W12" s="3" t="s">
         <v>300</v>
       </c>
       <c r="X12" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
@@ -7711,52 +7712,52 @@
         <v>76</v>
       </c>
       <c r="C13" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>697</v>
+        <v>707</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>203</v>
+        <v>121</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>241</v>
+        <v>123</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>232</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>673</v>
+        <v>683</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>203</v>
+        <v>121</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>241</v>
+        <v>123</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>232</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>326</v>
+        <v>284</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>282</v>
@@ -7774,903 +7775,1005 @@
         <v>302</v>
       </c>
       <c r="X13" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="1">
-        <v>4</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="W14" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="X14" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="1">
-        <v>4</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="X15" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="1">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>676</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="W16" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="X16" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="1">
-        <v>4</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="V17" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="W17" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="X17" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="1">
-        <v>5</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="W18" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="X18" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="1">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>679</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="W19" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="X19" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="1">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>704</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="W20" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="X20" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="1">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>705</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>681</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="W21" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="X21" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="1">
-        <v>6</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="W22" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="X22" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="1">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="W23" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="X23" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="1">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="U24" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="W24" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="X24" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="1">
-        <v>6</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>709</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="U25" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="V25" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="W25" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="X25" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:X13">
+    <sortCondition ref="C2:C13"/>
+    <sortCondition ref="D2:D13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6B8251-9C3F-BF40-8C4F-E253BBFC0ADC}">
+  <dimension ref="A1:X13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="A1:X13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="30.83203125" customWidth="1"/>
+    <col min="6" max="11" width="8.83203125" customWidth="1"/>
+    <col min="12" max="15" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:X13">
+    <sortCondition ref="C2:C13"/>
+    <sortCondition ref="D2:D13"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A91F786-6CEB-E344-8863-EBD0B851F207}">
   <dimension ref="A1:X13"/>
   <sheetViews>
@@ -9655,7 +9758,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C30D784-F3D0-A448-BA3E-DFEC988A722B}">
   <dimension ref="A1:W13"/>
   <sheetViews>
@@ -10601,7 +10704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5774199-2C1D-3246-99BA-868E98762941}">
   <dimension ref="A1:V13"/>
   <sheetViews>
@@ -11508,7 +11611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6937A4-C807-3848-96A3-22A225128EC7}">
   <dimension ref="A1:X13"/>
   <sheetViews>
@@ -12493,7 +12596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DD9CAC-B967-CA4E-8BD1-B1D66514996D}">
   <dimension ref="A1:V13"/>
   <sheetViews>
@@ -13390,913 +13493,6 @@
       </c>
       <c r="V13" s="3" t="s">
         <v>302</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A2:V13">
-    <sortCondition ref="C2:C13"/>
-    <sortCondition ref="D2:D13"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CBA894F-3BFE-6643-B5E2-96424F909891}">
-  <dimension ref="A1:V13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="14" width="5.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>842</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>830</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>843</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>839</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>844</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>831</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>845</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>832</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="2">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>846</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>833</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="2">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>847</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>834</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="2">
-        <v>4</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>848</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>835</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="2">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>849</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>840</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="U9" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="2">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>836</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="U10" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>851</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>837</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="U11" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="2">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>852</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>841</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="2">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>853</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>838</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -15257,6 +14453,913 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CBA894F-3BFE-6643-B5E2-96424F909891}">
+  <dimension ref="A1:V13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="14" width="5.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="2">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="2">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:V13">
+    <sortCondition ref="C2:C13"/>
+    <sortCondition ref="D2:D13"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58192B1F-C15B-3747-A3AA-546DBA5E9F9B}">
   <dimension ref="A1:U13"/>
   <sheetViews>
@@ -16124,7 +16227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23D747E-2E0A-104A-974F-1CEFD39DF9AB}">
   <dimension ref="A1:W13"/>
   <sheetViews>
@@ -17070,11 +17173,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD5108B-0EB4-7242-B1EC-BA2452F72B31}">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>

</xml_diff>